<commit_message>
LHCb data 8 TeV
</commit_message>
<xml_diff>
--- a/dy_qT/expdata/30001.xlsx
+++ b/dy_qT/expdata/30001.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/dy_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F2ABB605-327B-BE42-AE36-D7EEAF3700E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FD64AC-5703-5144-9643-B8E3F6F99786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2700" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="4280" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="30001" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
   <si>
     <t>FiducialCuts</t>
   </si>
@@ -98,12 +98,24 @@
   </si>
   <si>
     <t>pp-&gt;Z/gamma*-&gt;l+ l-</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>dsig/dpT</t>
+  </si>
+  <si>
+    <t>pb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -937,16 +949,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1016,8 +1028,14 @@
       <c r="W1" t="s">
         <v>23</v>
       </c>
+      <c r="X1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>13000</v>
       </c>
@@ -1087,8 +1105,14 @@
       <c r="W2" t="s">
         <v>25</v>
       </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13000</v>
       </c>
@@ -1158,8 +1182,14 @@
       <c r="W3" t="s">
         <v>25</v>
       </c>
+      <c r="X3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13000</v>
       </c>
@@ -1229,8 +1259,14 @@
       <c r="W4" t="s">
         <v>25</v>
       </c>
+      <c r="X4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13000</v>
       </c>
@@ -1300,8 +1336,14 @@
       <c r="W5" t="s">
         <v>25</v>
       </c>
+      <c r="X5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>13000</v>
       </c>
@@ -1371,8 +1413,14 @@
       <c r="W6" t="s">
         <v>25</v>
       </c>
+      <c r="X6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13000</v>
       </c>
@@ -1442,8 +1490,14 @@
       <c r="W7" t="s">
         <v>25</v>
       </c>
+      <c r="X7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>13000</v>
       </c>
@@ -1513,8 +1567,14 @@
       <c r="W8" t="s">
         <v>25</v>
       </c>
+      <c r="X8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>13000</v>
       </c>
@@ -1584,8 +1644,14 @@
       <c r="W9" t="s">
         <v>25</v>
       </c>
+      <c r="X9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>13000</v>
       </c>
@@ -1655,8 +1721,14 @@
       <c r="W10" t="s">
         <v>25</v>
       </c>
+      <c r="X10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>13000</v>
       </c>
@@ -1726,8 +1798,14 @@
       <c r="W11" t="s">
         <v>25</v>
       </c>
+      <c r="X11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13000</v>
       </c>
@@ -1797,8 +1875,14 @@
       <c r="W12" t="s">
         <v>25</v>
       </c>
+      <c r="X12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13000</v>
       </c>
@@ -1868,8 +1952,14 @@
       <c r="W13" t="s">
         <v>25</v>
       </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13000</v>
       </c>
@@ -1939,8 +2029,14 @@
       <c r="W14" t="s">
         <v>25</v>
       </c>
+      <c r="X14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13000</v>
       </c>
@@ -2009,6 +2105,12 @@
       </c>
       <c r="W15" t="s">
         <v>25</v>
+      </c>
+      <c r="X15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>